<commit_message>
attempting to commit after fixing github issues
</commit_message>
<xml_diff>
--- a/historical_data/historical_data_full.xlsx
+++ b/historical_data/historical_data_full.xlsx
@@ -3698,7 +3698,7 @@
         <v>133</v>
       </c>
       <c r="C265" t="n">
-        <v>41510.920997921</v>
+        <v>39744.5765595463</v>
       </c>
     </row>
   </sheetData>
@@ -6629,7 +6629,7 @@
         <v>133</v>
       </c>
       <c r="C265" t="n">
-        <v>1315.38085106383</v>
+        <v>1286.85575048733</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixing file pathways and updating Total Delta exports
</commit_message>
<xml_diff>
--- a/historical_data/historical_data_full.xlsx
+++ b/historical_data/historical_data_full.xlsx
@@ -3701,6 +3701,17 @@
         <v>38882.5045207957</v>
       </c>
     </row>
+    <row r="266">
+      <c r="A266" t="s">
+        <v>101</v>
+      </c>
+      <c r="B266" t="s">
+        <v>133</v>
+      </c>
+      <c r="C266" t="n">
+        <v>61946.510373444</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -6632,6 +6643,17 @@
         <v>1283.14606741573</v>
       </c>
     </row>
+    <row r="266">
+      <c r="A266" t="s">
+        <v>101</v>
+      </c>
+      <c r="B266" t="s">
+        <v>133</v>
+      </c>
+      <c r="C266" t="n">
+        <v>1161.95890410959</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -9550,6 +9572,17 @@
       </c>
       <c r="C264"/>
     </row>
+    <row r="265">
+      <c r="A265" t="s">
+        <v>101</v>
+      </c>
+      <c r="B265" t="s">
+        <v>133</v>
+      </c>
+      <c r="C265" t="n">
+        <v>6947</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
CVP and SWP updates
</commit_message>
<xml_diff>
--- a/historical_data/historical_data_full.xlsx
+++ b/historical_data/historical_data_full.xlsx
@@ -3709,7 +3709,7 @@
         <v>133</v>
       </c>
       <c r="C266" t="n">
-        <v>61946.510373444</v>
+        <v>64836.4121405751</v>
       </c>
     </row>
   </sheetData>
@@ -6651,7 +6651,7 @@
         <v>133</v>
       </c>
       <c r="C266" t="n">
-        <v>1161.95890410959</v>
+        <v>1199.46206896552</v>
       </c>
     </row>
   </sheetData>
@@ -9580,7 +9580,7 @@
         <v>133</v>
       </c>
       <c r="C265" t="n">
-        <v>6947</v>
+        <v>6754</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating maps to show legal delta border
</commit_message>
<xml_diff>
--- a/historical_data/historical_data_full.xlsx
+++ b/historical_data/historical_data_full.xlsx
@@ -3709,7 +3709,7 @@
         <v>133</v>
       </c>
       <c r="C266" t="n">
-        <v>64836.4121405751</v>
+        <v>67444.623556582</v>
       </c>
     </row>
   </sheetData>
@@ -6651,7 +6651,7 @@
         <v>133</v>
       </c>
       <c r="C266" t="n">
-        <v>1199.46206896552</v>
+        <v>1550.03201970443</v>
       </c>
     </row>
   </sheetData>
@@ -9580,7 +9580,7 @@
         <v>133</v>
       </c>
       <c r="C265" t="n">
-        <v>6754</v>
+        <v>6683</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding notes and making some lines of code more efficient by removing for loops and using expression finder
</commit_message>
<xml_diff>
--- a/historical_data/historical_data_full.xlsx
+++ b/historical_data/historical_data_full.xlsx
@@ -3709,7 +3709,7 @@
         <v>133</v>
       </c>
       <c r="C266" t="n">
-        <v>67444.623556582</v>
+        <v>67923.051975052</v>
       </c>
     </row>
   </sheetData>
@@ -6651,7 +6651,7 @@
         <v>133</v>
       </c>
       <c r="C266" t="n">
-        <v>1550.03201970443</v>
+        <v>1617.10154525386</v>
       </c>
     </row>
   </sheetData>
@@ -9580,7 +9580,7 @@
         <v>133</v>
       </c>
       <c r="C265" t="n">
-        <v>6683</v>
+        <v>6669</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding things to gitignore file
</commit_message>
<xml_diff>
--- a/historical_data/historical_data_full.xlsx
+++ b/historical_data/historical_data_full.xlsx
@@ -3712,6 +3712,17 @@
         <v>68260.4090121317</v>
       </c>
     </row>
+    <row r="267">
+      <c r="A267" t="s">
+        <v>135</v>
+      </c>
+      <c r="B267" t="s">
+        <v>133</v>
+      </c>
+      <c r="C267" t="n">
+        <v>50704.1020408163</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -6654,6 +6665,17 @@
         <v>1634.83941605839</v>
       </c>
     </row>
+    <row r="267">
+      <c r="A267" t="s">
+        <v>135</v>
+      </c>
+      <c r="B267" t="s">
+        <v>133</v>
+      </c>
+      <c r="C267" t="n">
+        <v>1533.44897959184</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -9583,6 +9605,17 @@
         <v>6639</v>
       </c>
     </row>
+    <row r="266">
+      <c r="A266" t="s">
+        <v>135</v>
+      </c>
+      <c r="B266" t="s">
+        <v>133</v>
+      </c>
+      <c r="C266" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
trying to fix git ignore
</commit_message>
<xml_diff>
--- a/historical_data/historical_data_full.xlsx
+++ b/historical_data/historical_data_full.xlsx
@@ -3720,7 +3720,7 @@
         <v>133</v>
       </c>
       <c r="C267" t="n">
-        <v>50704.1020408163</v>
+        <v>50255.0733944954</v>
       </c>
     </row>
   </sheetData>
@@ -6673,7 +6673,7 @@
         <v>133</v>
       </c>
       <c r="C267" t="n">
-        <v>1533.44897959184</v>
+        <v>1478.24827586207</v>
       </c>
     </row>
   </sheetData>
@@ -9613,7 +9613,7 @@
         <v>133</v>
       </c>
       <c r="C266" t="n">
-        <v>6086</v>
+        <v>6021</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating outputs with colors and fonts
</commit_message>
<xml_diff>
--- a/historical_data/historical_data_full.xlsx
+++ b/historical_data/historical_data_full.xlsx
@@ -3717,7 +3717,7 @@
         <v>132</v>
       </c>
       <c r="C268" t="n">
-        <v>50255.0733944954</v>
+        <v>46315.4498141264</v>
       </c>
     </row>
   </sheetData>
@@ -6679,7 +6679,7 @@
         <v>132</v>
       </c>
       <c r="C268" t="n">
-        <v>1683</v>
+        <v>2161.44827586207</v>
       </c>
     </row>
   </sheetData>
@@ -9637,7 +9637,7 @@
         <v>132</v>
       </c>
       <c r="C268" t="n">
-        <v>6148</v>
+        <v>6167</v>
       </c>
     </row>
   </sheetData>
@@ -12593,7 +12593,7 @@
         <v>132</v>
       </c>
       <c r="C268" t="n">
-        <v>47.2138408304498</v>
+        <v>47.2097713097713</v>
       </c>
     </row>
   </sheetData>
@@ -14847,7 +14847,7 @@
       </c>
       <c r="C187"/>
       <c r="D187" t="n">
-        <v>54.5742160278746</v>
+        <v>54.2279749478079</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added waterdrops images for the precipitation section
</commit_message>
<xml_diff>
--- a/historical_data/historical_data_full.xlsx
+++ b/historical_data/historical_data_full.xlsx
@@ -3584,7 +3584,7 @@
         <v>79</v>
       </c>
       <c r="C270" t="n">
-        <v>14004.2264150943</v>
+        <v>14085.8645833333</v>
       </c>
     </row>
   </sheetData>
@@ -6568,7 +6568,7 @@
         <v>79</v>
       </c>
       <c r="C270" t="n">
-        <v>2052.26037735849</v>
+        <v>1891.43636363636</v>
       </c>
     </row>
   </sheetData>
@@ -9548,7 +9548,7 @@
         <v>79</v>
       </c>
       <c r="C270" t="n">
-        <v>5703</v>
+        <v>5385</v>
       </c>
     </row>
   </sheetData>
@@ -12526,7 +12526,7 @@
         <v>79</v>
       </c>
       <c r="C270" t="n">
-        <v>57.2460377358491</v>
+        <v>56.1501298701299</v>
       </c>
     </row>
   </sheetData>
@@ -14804,7 +14804,7 @@
       </c>
       <c r="C189"/>
       <c r="D189" t="n">
-        <v>68.2750943396226</v>
+        <v>68.2007792207792</v>
       </c>
     </row>
   </sheetData>
@@ -17085,7 +17085,7 @@
       </c>
       <c r="C189"/>
       <c r="D189" t="n">
-        <v>74.6443773584906</v>
+        <v>74.343948051948</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changing graphs and adding color coding details
</commit_message>
<xml_diff>
--- a/historical_data/historical_data_full.xlsx
+++ b/historical_data/historical_data_full.xlsx
@@ -3584,7 +3584,7 @@
         <v>79</v>
       </c>
       <c r="C270" t="n">
-        <v>14085.8645833333</v>
+        <v>14303.2343387471</v>
       </c>
     </row>
   </sheetData>
@@ -6568,7 +6568,7 @@
         <v>79</v>
       </c>
       <c r="C270" t="n">
-        <v>1891.43636363636</v>
+        <v>1820.99769053118</v>
       </c>
     </row>
   </sheetData>
@@ -9548,7 +9548,7 @@
         <v>79</v>
       </c>
       <c r="C270" t="n">
-        <v>5385</v>
+        <v>5371</v>
       </c>
     </row>
   </sheetData>
@@ -12526,7 +12526,7 @@
         <v>79</v>
       </c>
       <c r="C270" t="n">
-        <v>56.1501298701299</v>
+        <v>55.8951501154734</v>
       </c>
     </row>
   </sheetData>
@@ -14804,7 +14804,7 @@
       </c>
       <c r="C189"/>
       <c r="D189" t="n">
-        <v>68.2007792207792</v>
+        <v>68.3110854503464</v>
       </c>
     </row>
   </sheetData>
@@ -17085,7 +17085,7 @@
       </c>
       <c r="C189"/>
       <c r="D189" t="n">
-        <v>74.343948051948</v>
+        <v>74.4533949191686</v>
       </c>
     </row>
   </sheetData>

</xml_diff>